<commit_message>
the app is almost done
</commit_message>
<xml_diff>
--- a/df_REFERENCE_PARAMETERS.xlsx
+++ b/df_REFERENCE_PARAMETERS.xlsx
@@ -684,7 +684,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Ammonium, ammonia</t>
+          <t>Ammonium and ammonia concentration parameters in water bodies</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -703,19 +703,19 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>2.27</v>
+        <v>90.28</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>61.11</v>
       </c>
       <c r="G7" t="n">
-        <v>9.09</v>
+        <v>100</v>
       </c>
       <c r="H7" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J7" t="n">
         <v>0</v>
@@ -7571,13 +7571,13 @@
         </is>
       </c>
       <c r="E179" t="n">
-        <v>4.54</v>
+        <v>25</v>
       </c>
       <c r="F179" t="n">
         <v>0</v>
       </c>
       <c r="G179" t="n">
-        <v>18.18</v>
+        <v>100</v>
       </c>
       <c r="H179" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
trying to solve the spatial coverage issue
</commit_message>
<xml_diff>
--- a/df_REFERENCE_PARAMETERS.xlsx
+++ b/df_REFERENCE_PARAMETERS.xlsx
@@ -1699,13 +1699,13 @@
         </is>
       </c>
       <c r="E32" t="n">
-        <v>52.27</v>
+        <v>50</v>
       </c>
       <c r="F32" t="n">
         <v>0</v>
       </c>
       <c r="G32" t="n">
-        <v>9.09</v>
+        <v>0</v>
       </c>
       <c r="H32" t="n">
         <v>100</v>

</xml_diff>

<commit_message>
fiking bugs and finishing codingthe Source data category
</commit_message>
<xml_diff>
--- a/df_REFERENCE_PARAMETERS.xlsx
+++ b/df_REFERENCE_PARAMETERS.xlsx
@@ -503,13 +503,13 @@
       </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="n">
-        <v>29.77</v>
+        <v>52.5</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>9.09</v>
+        <v>100</v>
       </c>
       <c r="H2" t="n">
         <v>10</v>
@@ -583,13 +583,13 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>34.77</v>
+        <v>39.32</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>9.09</v>
+        <v>27.27</v>
       </c>
       <c r="H4" t="n">
         <v>50</v>
@@ -623,13 +623,13 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>2.27</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>9.09</v>
+        <v>0</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
@@ -663,13 +663,13 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>2.27</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>9.09</v>
+        <v>0</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
@@ -743,13 +743,13 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>56.59</v>
+        <v>72.5</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>36.36</v>
+        <v>100</v>
       </c>
       <c r="H8" t="n">
         <v>100</v>
@@ -783,13 +783,13 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>59.09</v>
+        <v>75</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>36.36</v>
+        <v>100</v>
       </c>
       <c r="H9" t="n">
         <v>100</v>
@@ -823,13 +823,13 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>56.59</v>
+        <v>70.23</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>36.36</v>
+        <v>90.91</v>
       </c>
       <c r="H10" t="n">
         <v>100</v>
@@ -863,13 +863,13 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>67.42</v>
+        <v>83.33</v>
       </c>
       <c r="F11" t="n">
         <v>33.33</v>
       </c>
       <c r="G11" t="n">
-        <v>36.36</v>
+        <v>100</v>
       </c>
       <c r="H11" t="n">
         <v>100</v>
@@ -903,13 +903,13 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>56.59</v>
+        <v>61.14</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>36.36</v>
+        <v>54.55</v>
       </c>
       <c r="H12" t="n">
         <v>100</v>
@@ -943,13 +943,13 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>81.31</v>
+        <v>97.22</v>
       </c>
       <c r="F13" t="n">
         <v>88.89</v>
       </c>
       <c r="G13" t="n">
-        <v>36.36</v>
+        <v>100</v>
       </c>
       <c r="H13" t="n">
         <v>100</v>
@@ -979,13 +979,13 @@
       </c>
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="n">
-        <v>44.77</v>
+        <v>51.59</v>
       </c>
       <c r="F14" t="n">
         <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>9.09</v>
+        <v>36.36</v>
       </c>
       <c r="H14" t="n">
         <v>100</v>
@@ -1019,13 +1019,13 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>93.18000000000001</v>
+        <v>100</v>
       </c>
       <c r="F15" t="n">
         <v>100</v>
       </c>
       <c r="G15" t="n">
-        <v>72.73</v>
+        <v>100</v>
       </c>
       <c r="H15" t="n">
         <v>100</v>
@@ -1059,13 +1059,13 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>44.77</v>
+        <v>67.5</v>
       </c>
       <c r="F16" t="n">
         <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>9.09</v>
+        <v>100</v>
       </c>
       <c r="H16" t="n">
         <v>100</v>
@@ -1099,13 +1099,13 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>54.32</v>
+        <v>72.5</v>
       </c>
       <c r="F17" t="n">
         <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>27.27</v>
+        <v>100</v>
       </c>
       <c r="H17" t="n">
         <v>100</v>
@@ -1139,13 +1139,13 @@
         </is>
       </c>
       <c r="E18" t="n">
-        <v>70.45</v>
+        <v>75</v>
       </c>
       <c r="F18" t="n">
         <v>0</v>
       </c>
       <c r="G18" t="n">
-        <v>81.81999999999999</v>
+        <v>100</v>
       </c>
       <c r="H18" t="n">
         <v>100</v>
@@ -1179,13 +1179,13 @@
         </is>
       </c>
       <c r="E19" t="n">
-        <v>56.82</v>
+        <v>75</v>
       </c>
       <c r="F19" t="n">
         <v>0</v>
       </c>
       <c r="G19" t="n">
-        <v>27.27</v>
+        <v>100</v>
       </c>
       <c r="H19" t="n">
         <v>100</v>
@@ -1219,13 +1219,13 @@
         </is>
       </c>
       <c r="E20" t="n">
-        <v>56.82</v>
+        <v>75</v>
       </c>
       <c r="F20" t="n">
         <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>27.27</v>
+        <v>100</v>
       </c>
       <c r="H20" t="n">
         <v>100</v>
@@ -1339,13 +1339,13 @@
         </is>
       </c>
       <c r="E23" t="n">
-        <v>61.36</v>
+        <v>75</v>
       </c>
       <c r="F23" t="n">
         <v>0</v>
       </c>
       <c r="G23" t="n">
-        <v>45.45</v>
+        <v>100</v>
       </c>
       <c r="H23" t="n">
         <v>100</v>
@@ -1379,13 +1379,13 @@
         </is>
       </c>
       <c r="E24" t="n">
-        <v>58.86</v>
+        <v>72.5</v>
       </c>
       <c r="F24" t="n">
         <v>0</v>
       </c>
       <c r="G24" t="n">
-        <v>45.45</v>
+        <v>100</v>
       </c>
       <c r="H24" t="n">
         <v>100</v>
@@ -1419,13 +1419,13 @@
         </is>
       </c>
       <c r="E25" t="n">
-        <v>58.86</v>
+        <v>72.5</v>
       </c>
       <c r="F25" t="n">
         <v>0</v>
       </c>
       <c r="G25" t="n">
-        <v>45.45</v>
+        <v>100</v>
       </c>
       <c r="H25" t="n">
         <v>100</v>
@@ -1459,13 +1459,13 @@
         </is>
       </c>
       <c r="E26" t="n">
-        <v>58.86</v>
+        <v>72.5</v>
       </c>
       <c r="F26" t="n">
         <v>0</v>
       </c>
       <c r="G26" t="n">
-        <v>45.45</v>
+        <v>100</v>
       </c>
       <c r="H26" t="n">
         <v>100</v>
@@ -1499,13 +1499,13 @@
         </is>
       </c>
       <c r="E27" t="n">
-        <v>58.86</v>
+        <v>72.5</v>
       </c>
       <c r="F27" t="n">
         <v>0</v>
       </c>
       <c r="G27" t="n">
-        <v>45.45</v>
+        <v>100</v>
       </c>
       <c r="H27" t="n">
         <v>100</v>
@@ -1699,13 +1699,13 @@
         </is>
       </c>
       <c r="E32" t="n">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="F32" t="n">
         <v>0</v>
       </c>
       <c r="G32" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="H32" t="n">
         <v>100</v>
@@ -1779,13 +1779,13 @@
         </is>
       </c>
       <c r="E34" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="F34" t="n">
         <v>0</v>
       </c>
       <c r="G34" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H34" t="n">
         <v>0</v>
@@ -1859,13 +1859,13 @@
         </is>
       </c>
       <c r="E36" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="F36" t="n">
         <v>0</v>
       </c>
       <c r="G36" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H36" t="n">
         <v>0</v>
@@ -1939,13 +1939,13 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>83.59</v>
+        <v>97.22</v>
       </c>
       <c r="F38" t="n">
         <v>88.89</v>
       </c>
       <c r="G38" t="n">
-        <v>45.45</v>
+        <v>100</v>
       </c>
       <c r="H38" t="n">
         <v>100</v>
@@ -1979,13 +1979,13 @@
         </is>
       </c>
       <c r="E39" t="n">
-        <v>42.27</v>
+        <v>65</v>
       </c>
       <c r="F39" t="n">
         <v>0</v>
       </c>
       <c r="G39" t="n">
-        <v>9.09</v>
+        <v>100</v>
       </c>
       <c r="H39" t="n">
         <v>100</v>
@@ -2019,13 +2019,13 @@
         </is>
       </c>
       <c r="E40" t="n">
-        <v>60.68</v>
+        <v>67.5</v>
       </c>
       <c r="F40" t="n">
         <v>0</v>
       </c>
       <c r="G40" t="n">
-        <v>72.73</v>
+        <v>100</v>
       </c>
       <c r="H40" t="n">
         <v>100</v>
@@ -2099,13 +2099,13 @@
         </is>
       </c>
       <c r="E42" t="n">
-        <v>65.23</v>
+        <v>67.5</v>
       </c>
       <c r="F42" t="n">
         <v>0</v>
       </c>
       <c r="G42" t="n">
-        <v>90.91</v>
+        <v>100</v>
       </c>
       <c r="H42" t="n">
         <v>100</v>
@@ -2139,13 +2139,13 @@
         </is>
       </c>
       <c r="E43" t="n">
-        <v>52.27</v>
+        <v>75</v>
       </c>
       <c r="F43" t="n">
         <v>0</v>
       </c>
       <c r="G43" t="n">
-        <v>9.09</v>
+        <v>100</v>
       </c>
       <c r="H43" t="n">
         <v>100</v>
@@ -2179,13 +2179,13 @@
         </is>
       </c>
       <c r="E44" t="n">
-        <v>2.27</v>
+        <v>0</v>
       </c>
       <c r="F44" t="n">
         <v>0</v>
       </c>
       <c r="G44" t="n">
-        <v>9.09</v>
+        <v>0</v>
       </c>
       <c r="H44" t="n">
         <v>0</v>
@@ -2259,13 +2259,13 @@
         </is>
       </c>
       <c r="E46" t="n">
-        <v>58.18</v>
+        <v>65</v>
       </c>
       <c r="F46" t="n">
         <v>0</v>
       </c>
       <c r="G46" t="n">
-        <v>72.73</v>
+        <v>100</v>
       </c>
       <c r="H46" t="n">
         <v>100</v>
@@ -2419,13 +2419,13 @@
         </is>
       </c>
       <c r="E50" t="n">
-        <v>65.68000000000001</v>
+        <v>72.5</v>
       </c>
       <c r="F50" t="n">
         <v>0</v>
       </c>
       <c r="G50" t="n">
-        <v>72.73</v>
+        <v>100</v>
       </c>
       <c r="H50" t="n">
         <v>100</v>
@@ -2619,13 +2619,13 @@
         </is>
       </c>
       <c r="E55" t="n">
-        <v>42.27</v>
+        <v>58.18</v>
       </c>
       <c r="F55" t="n">
         <v>0</v>
       </c>
       <c r="G55" t="n">
-        <v>9.09</v>
+        <v>72.73</v>
       </c>
       <c r="H55" t="n">
         <v>100</v>
@@ -2659,13 +2659,13 @@
         </is>
       </c>
       <c r="E56" t="n">
-        <v>2.27</v>
+        <v>0</v>
       </c>
       <c r="F56" t="n">
         <v>0</v>
       </c>
       <c r="G56" t="n">
-        <v>9.09</v>
+        <v>0</v>
       </c>
       <c r="H56" t="n">
         <v>0</v>
@@ -2699,13 +2699,13 @@
         </is>
       </c>
       <c r="E57" t="n">
-        <v>29.77</v>
+        <v>52.5</v>
       </c>
       <c r="F57" t="n">
         <v>0</v>
       </c>
       <c r="G57" t="n">
-        <v>9.09</v>
+        <v>100</v>
       </c>
       <c r="H57" t="n">
         <v>30</v>
@@ -2735,13 +2735,13 @@
       </c>
       <c r="D58" t="inlineStr"/>
       <c r="E58" t="n">
-        <v>59.22</v>
+        <v>81.94</v>
       </c>
       <c r="F58" t="n">
         <v>27.78</v>
       </c>
       <c r="G58" t="n">
-        <v>9.09</v>
+        <v>100</v>
       </c>
       <c r="H58" t="n">
         <v>100</v>
@@ -2855,13 +2855,13 @@
         </is>
       </c>
       <c r="E61" t="n">
-        <v>68.31</v>
+        <v>81.94</v>
       </c>
       <c r="F61" t="n">
         <v>27.78</v>
       </c>
       <c r="G61" t="n">
-        <v>45.45</v>
+        <v>100</v>
       </c>
       <c r="H61" t="n">
         <v>100</v>
@@ -3095,13 +3095,13 @@
         </is>
       </c>
       <c r="E67" t="n">
-        <v>54.32</v>
+        <v>72.5</v>
       </c>
       <c r="F67" t="n">
         <v>0</v>
       </c>
       <c r="G67" t="n">
-        <v>27.27</v>
+        <v>100</v>
       </c>
       <c r="H67" t="n">
         <v>100</v>
@@ -3175,13 +3175,13 @@
         </is>
       </c>
       <c r="E69" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="F69" t="n">
         <v>0</v>
       </c>
       <c r="G69" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H69" t="n">
         <v>0</v>
@@ -3215,13 +3215,13 @@
         </is>
       </c>
       <c r="E70" t="n">
-        <v>59.09</v>
+        <v>75</v>
       </c>
       <c r="F70" t="n">
         <v>0</v>
       </c>
       <c r="G70" t="n">
-        <v>36.36</v>
+        <v>100</v>
       </c>
       <c r="H70" t="n">
         <v>100</v>
@@ -3255,13 +3255,13 @@
         </is>
       </c>
       <c r="E71" t="n">
-        <v>59.09</v>
+        <v>75</v>
       </c>
       <c r="F71" t="n">
         <v>0</v>
       </c>
       <c r="G71" t="n">
-        <v>36.36</v>
+        <v>100</v>
       </c>
       <c r="H71" t="n">
         <v>100</v>
@@ -3335,13 +3335,13 @@
         </is>
       </c>
       <c r="E73" t="n">
-        <v>70.45</v>
+        <v>75</v>
       </c>
       <c r="F73" t="n">
         <v>0</v>
       </c>
       <c r="G73" t="n">
-        <v>81.81999999999999</v>
+        <v>100</v>
       </c>
       <c r="H73" t="n">
         <v>100</v>
@@ -3415,13 +3415,13 @@
         </is>
       </c>
       <c r="E75" t="n">
-        <v>52.27</v>
+        <v>75</v>
       </c>
       <c r="F75" t="n">
         <v>0</v>
       </c>
       <c r="G75" t="n">
-        <v>9.09</v>
+        <v>100</v>
       </c>
       <c r="H75" t="n">
         <v>100</v>
@@ -3455,13 +3455,13 @@
         </is>
       </c>
       <c r="E76" t="n">
-        <v>59.09</v>
+        <v>75</v>
       </c>
       <c r="F76" t="n">
         <v>0</v>
       </c>
       <c r="G76" t="n">
-        <v>36.36</v>
+        <v>100</v>
       </c>
       <c r="H76" t="n">
         <v>100</v>
@@ -3495,13 +3495,13 @@
         </is>
       </c>
       <c r="E77" t="n">
-        <v>59.09</v>
+        <v>75</v>
       </c>
       <c r="F77" t="n">
         <v>0</v>
       </c>
       <c r="G77" t="n">
-        <v>36.36</v>
+        <v>100</v>
       </c>
       <c r="H77" t="n">
         <v>100</v>
@@ -3615,13 +3615,13 @@
         </is>
       </c>
       <c r="E80" t="n">
-        <v>35.88</v>
+        <v>51.79</v>
       </c>
       <c r="F80" t="n">
         <v>94.44</v>
       </c>
       <c r="G80" t="n">
-        <v>9.09</v>
+        <v>72.73</v>
       </c>
       <c r="H80" t="n">
         <v>0</v>
@@ -3655,13 +3655,13 @@
         </is>
       </c>
       <c r="E81" t="n">
-        <v>67.27</v>
+        <v>90</v>
       </c>
       <c r="F81" t="n">
         <v>100</v>
       </c>
       <c r="G81" t="n">
-        <v>9.09</v>
+        <v>100</v>
       </c>
       <c r="H81" t="n">
         <v>100</v>
@@ -3695,13 +3695,13 @@
         </is>
       </c>
       <c r="E82" t="n">
-        <v>67.27</v>
+        <v>90</v>
       </c>
       <c r="F82" t="n">
         <v>100</v>
       </c>
       <c r="G82" t="n">
-        <v>9.09</v>
+        <v>100</v>
       </c>
       <c r="H82" t="n">
         <v>100</v>
@@ -3855,13 +3855,13 @@
         </is>
       </c>
       <c r="E86" t="n">
-        <v>45.68</v>
+        <v>52.5</v>
       </c>
       <c r="F86" t="n">
         <v>0</v>
       </c>
       <c r="G86" t="n">
-        <v>72.73</v>
+        <v>100</v>
       </c>
       <c r="H86" t="n">
         <v>30</v>
@@ -3895,13 +3895,13 @@
         </is>
       </c>
       <c r="E87" t="n">
-        <v>65.68000000000001</v>
+        <v>72.5</v>
       </c>
       <c r="F87" t="n">
         <v>0</v>
       </c>
       <c r="G87" t="n">
-        <v>72.73</v>
+        <v>100</v>
       </c>
       <c r="H87" t="n">
         <v>100</v>
@@ -3935,13 +3935,13 @@
         </is>
       </c>
       <c r="E88" t="n">
-        <v>77.14</v>
+        <v>93.06</v>
       </c>
       <c r="F88" t="n">
         <v>72.22</v>
       </c>
       <c r="G88" t="n">
-        <v>36.36</v>
+        <v>100</v>
       </c>
       <c r="H88" t="n">
         <v>100</v>
@@ -4055,13 +4055,13 @@
         </is>
       </c>
       <c r="E91" t="n">
-        <v>70.58</v>
+        <v>81.94</v>
       </c>
       <c r="F91" t="n">
         <v>27.78</v>
       </c>
       <c r="G91" t="n">
-        <v>54.55</v>
+        <v>100</v>
       </c>
       <c r="H91" t="n">
         <v>100</v>
@@ -4175,13 +4175,13 @@
         </is>
       </c>
       <c r="E94" t="n">
-        <v>68.18000000000001</v>
+        <v>75</v>
       </c>
       <c r="F94" t="n">
         <v>0</v>
       </c>
       <c r="G94" t="n">
-        <v>72.73</v>
+        <v>100</v>
       </c>
       <c r="H94" t="n">
         <v>100</v>
@@ -4215,13 +4215,13 @@
         </is>
       </c>
       <c r="E95" t="n">
-        <v>59.04</v>
+        <v>77.22</v>
       </c>
       <c r="F95" t="n">
         <v>88.89</v>
       </c>
       <c r="G95" t="n">
-        <v>27.27</v>
+        <v>100</v>
       </c>
       <c r="H95" t="n">
         <v>20</v>
@@ -4255,13 +4255,13 @@
         </is>
       </c>
       <c r="E96" t="n">
-        <v>74.5</v>
+        <v>97.22</v>
       </c>
       <c r="F96" t="n">
         <v>88.89</v>
       </c>
       <c r="G96" t="n">
-        <v>9.09</v>
+        <v>100</v>
       </c>
       <c r="H96" t="n">
         <v>100</v>
@@ -4335,13 +4335,13 @@
         </is>
       </c>
       <c r="E98" t="n">
-        <v>56.44</v>
+        <v>79.17</v>
       </c>
       <c r="F98" t="n">
         <v>16.67</v>
       </c>
       <c r="G98" t="n">
-        <v>9.09</v>
+        <v>100</v>
       </c>
       <c r="H98" t="n">
         <v>100</v>
@@ -4375,13 +4375,13 @@
         </is>
       </c>
       <c r="E99" t="n">
-        <v>2.27</v>
+        <v>0</v>
       </c>
       <c r="F99" t="n">
         <v>0</v>
       </c>
       <c r="G99" t="n">
-        <v>9.09</v>
+        <v>0</v>
       </c>
       <c r="H99" t="n">
         <v>0</v>
@@ -4415,13 +4415,13 @@
         </is>
       </c>
       <c r="E100" t="n">
-        <v>60.68</v>
+        <v>67.5</v>
       </c>
       <c r="F100" t="n">
         <v>0</v>
       </c>
       <c r="G100" t="n">
-        <v>72.73</v>
+        <v>100</v>
       </c>
       <c r="H100" t="n">
         <v>100</v>
@@ -4535,13 +4535,13 @@
         </is>
       </c>
       <c r="E103" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="F103" t="n">
         <v>0</v>
       </c>
       <c r="G103" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H103" t="n">
         <v>0</v>
@@ -4771,13 +4771,13 @@
         </is>
       </c>
       <c r="E109" t="n">
-        <v>65.68000000000001</v>
+        <v>72.5</v>
       </c>
       <c r="F109" t="n">
         <v>0</v>
       </c>
       <c r="G109" t="n">
-        <v>72.73</v>
+        <v>100</v>
       </c>
       <c r="H109" t="n">
         <v>100</v>
@@ -4811,13 +4811,13 @@
         </is>
       </c>
       <c r="E110" t="n">
-        <v>65.68000000000001</v>
+        <v>72.5</v>
       </c>
       <c r="F110" t="n">
         <v>0</v>
       </c>
       <c r="G110" t="n">
-        <v>72.73</v>
+        <v>100</v>
       </c>
       <c r="H110" t="n">
         <v>100</v>
@@ -4851,13 +4851,13 @@
         </is>
       </c>
       <c r="E111" t="n">
-        <v>65.68000000000001</v>
+        <v>72.5</v>
       </c>
       <c r="F111" t="n">
         <v>0</v>
       </c>
       <c r="G111" t="n">
-        <v>72.73</v>
+        <v>100</v>
       </c>
       <c r="H111" t="n">
         <v>100</v>
@@ -5091,13 +5091,13 @@
         </is>
       </c>
       <c r="E117" t="n">
-        <v>80.43000000000001</v>
+        <v>98.61</v>
       </c>
       <c r="F117" t="n">
         <v>94.44</v>
       </c>
       <c r="G117" t="n">
-        <v>27.27</v>
+        <v>100</v>
       </c>
       <c r="H117" t="n">
         <v>100</v>
@@ -5131,13 +5131,13 @@
         </is>
       </c>
       <c r="E118" t="n">
-        <v>80.43000000000001</v>
+        <v>98.61</v>
       </c>
       <c r="F118" t="n">
         <v>94.44</v>
       </c>
       <c r="G118" t="n">
-        <v>27.27</v>
+        <v>100</v>
       </c>
       <c r="H118" t="n">
         <v>100</v>
@@ -5251,13 +5251,13 @@
         </is>
       </c>
       <c r="E121" t="n">
-        <v>63.41</v>
+        <v>72.5</v>
       </c>
       <c r="F121" t="n">
         <v>0</v>
       </c>
       <c r="G121" t="n">
-        <v>63.64</v>
+        <v>100</v>
       </c>
       <c r="H121" t="n">
         <v>100</v>
@@ -5291,13 +5291,13 @@
         </is>
       </c>
       <c r="E122" t="n">
-        <v>62.73</v>
+        <v>65</v>
       </c>
       <c r="F122" t="n">
         <v>0</v>
       </c>
       <c r="G122" t="n">
-        <v>90.91</v>
+        <v>100</v>
       </c>
       <c r="H122" t="n">
         <v>100</v>
@@ -5371,13 +5371,13 @@
         </is>
       </c>
       <c r="E124" t="n">
-        <v>77.53</v>
+        <v>88.89</v>
       </c>
       <c r="F124" t="n">
         <v>55.56</v>
       </c>
       <c r="G124" t="n">
-        <v>54.55</v>
+        <v>100</v>
       </c>
       <c r="H124" t="n">
         <v>100</v>
@@ -5451,13 +5451,13 @@
         </is>
       </c>
       <c r="E126" t="n">
-        <v>68.18000000000001</v>
+        <v>75</v>
       </c>
       <c r="F126" t="n">
         <v>0</v>
       </c>
       <c r="G126" t="n">
-        <v>72.73</v>
+        <v>100</v>
       </c>
       <c r="H126" t="n">
         <v>100</v>
@@ -5971,13 +5971,13 @@
         </is>
       </c>
       <c r="E139" t="n">
-        <v>74.75</v>
+        <v>86.11</v>
       </c>
       <c r="F139" t="n">
         <v>44.44</v>
       </c>
       <c r="G139" t="n">
-        <v>54.55</v>
+        <v>100</v>
       </c>
       <c r="H139" t="n">
         <v>100</v>
@@ -6171,10 +6171,10 @@
         </is>
       </c>
       <c r="E144" t="n">
-        <v>83.33</v>
+        <v>81.94</v>
       </c>
       <c r="F144" t="n">
-        <v>33.33</v>
+        <v>27.78</v>
       </c>
       <c r="G144" t="n">
         <v>100</v>
@@ -6211,13 +6211,13 @@
         </is>
       </c>
       <c r="E145" t="n">
-        <v>39.32</v>
+        <v>41.59</v>
       </c>
       <c r="F145" t="n">
         <v>0</v>
       </c>
       <c r="G145" t="n">
-        <v>27.27</v>
+        <v>36.36</v>
       </c>
       <c r="H145" t="n">
         <v>50</v>
@@ -6251,13 +6251,13 @@
         </is>
       </c>
       <c r="E146" t="n">
-        <v>6.82</v>
+        <v>0</v>
       </c>
       <c r="F146" t="n">
         <v>0</v>
       </c>
       <c r="G146" t="n">
-        <v>27.27</v>
+        <v>0</v>
       </c>
       <c r="H146" t="n">
         <v>0</v>
@@ -6331,13 +6331,13 @@
         </is>
       </c>
       <c r="E148" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="F148" t="n">
         <v>0</v>
       </c>
       <c r="G148" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H148" t="n">
         <v>0</v>
@@ -6371,13 +6371,13 @@
         </is>
       </c>
       <c r="E149" t="n">
-        <v>70.33</v>
+        <v>93.06</v>
       </c>
       <c r="F149" t="n">
         <v>72.22</v>
       </c>
       <c r="G149" t="n">
-        <v>9.09</v>
+        <v>100</v>
       </c>
       <c r="H149" t="n">
         <v>100</v>
@@ -6411,13 +6411,13 @@
         </is>
       </c>
       <c r="E150" t="n">
-        <v>69.77</v>
+        <v>92.5</v>
       </c>
       <c r="F150" t="n">
         <v>100</v>
       </c>
       <c r="G150" t="n">
-        <v>9.09</v>
+        <v>100</v>
       </c>
       <c r="H150" t="n">
         <v>100</v>
@@ -6491,13 +6491,13 @@
         </is>
       </c>
       <c r="E152" t="n">
-        <v>68.18000000000001</v>
+        <v>75</v>
       </c>
       <c r="F152" t="n">
         <v>0</v>
       </c>
       <c r="G152" t="n">
-        <v>72.73</v>
+        <v>100</v>
       </c>
       <c r="H152" t="n">
         <v>100</v>
@@ -6531,13 +6531,13 @@
         </is>
       </c>
       <c r="E153" t="n">
-        <v>65.68000000000001</v>
+        <v>72.5</v>
       </c>
       <c r="F153" t="n">
         <v>0</v>
       </c>
       <c r="G153" t="n">
-        <v>72.73</v>
+        <v>100</v>
       </c>
       <c r="H153" t="n">
         <v>100</v>
@@ -6571,13 +6571,13 @@
         </is>
       </c>
       <c r="E154" t="n">
-        <v>65.68000000000001</v>
+        <v>72.5</v>
       </c>
       <c r="F154" t="n">
         <v>0</v>
       </c>
       <c r="G154" t="n">
-        <v>72.73</v>
+        <v>100</v>
       </c>
       <c r="H154" t="n">
         <v>100</v>
@@ -6611,13 +6611,13 @@
         </is>
       </c>
       <c r="E155" t="n">
-        <v>68.18000000000001</v>
+        <v>75</v>
       </c>
       <c r="F155" t="n">
         <v>0</v>
       </c>
       <c r="G155" t="n">
-        <v>72.73</v>
+        <v>100</v>
       </c>
       <c r="H155" t="n">
         <v>100</v>
@@ -6651,13 +6651,13 @@
         </is>
       </c>
       <c r="E156" t="n">
-        <v>68.18000000000001</v>
+        <v>75</v>
       </c>
       <c r="F156" t="n">
         <v>0</v>
       </c>
       <c r="G156" t="n">
-        <v>72.73</v>
+        <v>100</v>
       </c>
       <c r="H156" t="n">
         <v>100</v>
@@ -6691,13 +6691,13 @@
         </is>
       </c>
       <c r="E157" t="n">
-        <v>72.34999999999999</v>
+        <v>79.17</v>
       </c>
       <c r="F157" t="n">
         <v>16.67</v>
       </c>
       <c r="G157" t="n">
-        <v>72.73</v>
+        <v>100</v>
       </c>
       <c r="H157" t="n">
         <v>100</v>
@@ -6771,13 +6771,13 @@
         </is>
       </c>
       <c r="E159" t="n">
-        <v>44.55</v>
+        <v>46.82</v>
       </c>
       <c r="F159" t="n">
         <v>0</v>
       </c>
       <c r="G159" t="n">
-        <v>18.18</v>
+        <v>27.27</v>
       </c>
       <c r="H159" t="n">
         <v>100</v>
@@ -6811,13 +6811,13 @@
         </is>
       </c>
       <c r="E160" t="n">
-        <v>4.54</v>
+        <v>0</v>
       </c>
       <c r="F160" t="n">
         <v>0</v>
       </c>
       <c r="G160" t="n">
-        <v>18.18</v>
+        <v>0</v>
       </c>
       <c r="H160" t="n">
         <v>0</v>
@@ -6851,13 +6851,13 @@
         </is>
       </c>
       <c r="E161" t="n">
-        <v>67.27</v>
+        <v>90</v>
       </c>
       <c r="F161" t="n">
         <v>100</v>
       </c>
       <c r="G161" t="n">
-        <v>9.09</v>
+        <v>100</v>
       </c>
       <c r="H161" t="n">
         <v>100</v>
@@ -6931,13 +6931,13 @@
         </is>
       </c>
       <c r="E163" t="n">
-        <v>52.27</v>
+        <v>68.18000000000001</v>
       </c>
       <c r="F163" t="n">
         <v>100</v>
       </c>
       <c r="G163" t="n">
-        <v>9.09</v>
+        <v>72.73</v>
       </c>
       <c r="H163" t="n">
         <v>60</v>
@@ -6971,13 +6971,13 @@
         </is>
       </c>
       <c r="E164" t="n">
-        <v>52.27</v>
+        <v>75</v>
       </c>
       <c r="F164" t="n">
         <v>100</v>
       </c>
       <c r="G164" t="n">
-        <v>9.09</v>
+        <v>100</v>
       </c>
       <c r="H164" t="n">
         <v>60</v>
@@ -7011,13 +7011,13 @@
         </is>
       </c>
       <c r="E165" t="n">
-        <v>2.27</v>
+        <v>0</v>
       </c>
       <c r="F165" t="n">
         <v>0</v>
       </c>
       <c r="G165" t="n">
-        <v>9.09</v>
+        <v>0</v>
       </c>
       <c r="H165" t="n">
         <v>0</v>
@@ -7051,13 +7051,13 @@
         </is>
       </c>
       <c r="E166" t="n">
-        <v>72.05</v>
+        <v>92.5</v>
       </c>
       <c r="F166" t="n">
         <v>100</v>
       </c>
       <c r="G166" t="n">
-        <v>18.18</v>
+        <v>100</v>
       </c>
       <c r="H166" t="n">
         <v>100</v>
@@ -7131,13 +7131,13 @@
         </is>
       </c>
       <c r="E168" t="n">
-        <v>78.16</v>
+        <v>98.61</v>
       </c>
       <c r="F168" t="n">
         <v>94.44</v>
       </c>
       <c r="G168" t="n">
-        <v>18.18</v>
+        <v>100</v>
       </c>
       <c r="H168" t="n">
         <v>100</v>
@@ -7171,13 +7171,13 @@
         </is>
       </c>
       <c r="E169" t="n">
-        <v>52.27</v>
+        <v>68.18000000000001</v>
       </c>
       <c r="F169" t="n">
         <v>100</v>
       </c>
       <c r="G169" t="n">
-        <v>9.09</v>
+        <v>72.73</v>
       </c>
       <c r="H169" t="n">
         <v>60</v>
@@ -7211,13 +7211,13 @@
         </is>
       </c>
       <c r="E170" t="n">
-        <v>52.27</v>
+        <v>68.18000000000001</v>
       </c>
       <c r="F170" t="n">
         <v>100</v>
       </c>
       <c r="G170" t="n">
-        <v>9.09</v>
+        <v>72.73</v>
       </c>
       <c r="H170" t="n">
         <v>60</v>
@@ -7251,13 +7251,13 @@
         </is>
       </c>
       <c r="E171" t="n">
-        <v>61.36</v>
+        <v>75</v>
       </c>
       <c r="F171" t="n">
         <v>0</v>
       </c>
       <c r="G171" t="n">
-        <v>45.45</v>
+        <v>100</v>
       </c>
       <c r="H171" t="n">
         <v>100</v>
@@ -7291,13 +7291,13 @@
         </is>
       </c>
       <c r="E172" t="n">
-        <v>11.36</v>
+        <v>0</v>
       </c>
       <c r="F172" t="n">
         <v>0</v>
       </c>
       <c r="G172" t="n">
-        <v>45.45</v>
+        <v>0</v>
       </c>
       <c r="H172" t="n">
         <v>0</v>
@@ -7371,13 +7371,13 @@
         </is>
       </c>
       <c r="E174" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="F174" t="n">
         <v>0</v>
       </c>
       <c r="G174" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H174" t="n">
         <v>0</v>
@@ -7411,13 +7411,13 @@
         </is>
       </c>
       <c r="E175" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="F175" t="n">
         <v>0</v>
       </c>
       <c r="G175" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H175" t="n">
         <v>0</v>
@@ -7451,13 +7451,13 @@
         </is>
       </c>
       <c r="E176" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="F176" t="n">
         <v>0</v>
       </c>
       <c r="G176" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H176" t="n">
         <v>0</v>
@@ -7571,13 +7571,13 @@
         </is>
       </c>
       <c r="E179" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="F179" t="n">
         <v>0</v>
       </c>
       <c r="G179" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H179" t="n">
         <v>0</v>
@@ -7691,13 +7691,13 @@
         </is>
       </c>
       <c r="E182" t="n">
-        <v>89.52</v>
+        <v>98.61</v>
       </c>
       <c r="F182" t="n">
         <v>94.44</v>
       </c>
       <c r="G182" t="n">
-        <v>63.64</v>
+        <v>100</v>
       </c>
       <c r="H182" t="n">
         <v>100</v>
@@ -7891,13 +7891,13 @@
         </is>
       </c>
       <c r="E187" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="F187" t="n">
         <v>0</v>
       </c>
       <c r="G187" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H187" t="n">
         <v>0</v>
@@ -8011,13 +8011,13 @@
         </is>
       </c>
       <c r="E190" t="n">
-        <v>56.36</v>
+        <v>70</v>
       </c>
       <c r="F190" t="n">
         <v>0</v>
       </c>
       <c r="G190" t="n">
-        <v>45.45</v>
+        <v>100</v>
       </c>
       <c r="H190" t="n">
         <v>100</v>
@@ -8211,13 +8211,13 @@
         </is>
       </c>
       <c r="E195" t="n">
-        <v>72.73</v>
+        <v>75</v>
       </c>
       <c r="F195" t="n">
         <v>0</v>
       </c>
       <c r="G195" t="n">
-        <v>90.91</v>
+        <v>100</v>
       </c>
       <c r="H195" t="n">
         <v>100</v>
@@ -8251,13 +8251,13 @@
         </is>
       </c>
       <c r="E196" t="n">
-        <v>77.65000000000001</v>
+        <v>95.83</v>
       </c>
       <c r="F196" t="n">
         <v>83.33</v>
       </c>
       <c r="G196" t="n">
-        <v>27.27</v>
+        <v>100</v>
       </c>
       <c r="H196" t="n">
         <v>100</v>
@@ -8291,13 +8291,13 @@
         </is>
       </c>
       <c r="E197" t="n">
-        <v>59.22</v>
+        <v>81.94</v>
       </c>
       <c r="F197" t="n">
         <v>27.78</v>
       </c>
       <c r="G197" t="n">
-        <v>9.09</v>
+        <v>100</v>
       </c>
       <c r="H197" t="n">
         <v>100</v>
@@ -8331,13 +8331,13 @@
         </is>
       </c>
       <c r="E198" t="n">
-        <v>73.11</v>
+        <v>95.83</v>
       </c>
       <c r="F198" t="n">
         <v>83.33</v>
       </c>
       <c r="G198" t="n">
-        <v>9.09</v>
+        <v>100</v>
       </c>
       <c r="H198" t="n">
         <v>100</v>
@@ -8371,13 +8371,13 @@
         </is>
       </c>
       <c r="E199" t="n">
-        <v>60.61</v>
+        <v>83.33</v>
       </c>
       <c r="F199" t="n">
         <v>33.33</v>
       </c>
       <c r="G199" t="n">
-        <v>9.09</v>
+        <v>100</v>
       </c>
       <c r="H199" t="n">
         <v>100</v>
@@ -8411,13 +8411,13 @@
         </is>
       </c>
       <c r="E200" t="n">
-        <v>59.22</v>
+        <v>81.94</v>
       </c>
       <c r="F200" t="n">
         <v>27.78</v>
       </c>
       <c r="G200" t="n">
-        <v>9.09</v>
+        <v>100</v>
       </c>
       <c r="H200" t="n">
         <v>100</v>
@@ -8451,13 +8451,13 @@
         </is>
       </c>
       <c r="E201" t="n">
-        <v>54.09</v>
+        <v>70</v>
       </c>
       <c r="F201" t="n">
         <v>0</v>
       </c>
       <c r="G201" t="n">
-        <v>36.36</v>
+        <v>100</v>
       </c>
       <c r="H201" t="n">
         <v>100</v>
@@ -8491,13 +8491,13 @@
         </is>
       </c>
       <c r="E202" t="n">
-        <v>56.59</v>
+        <v>72.5</v>
       </c>
       <c r="F202" t="n">
         <v>0</v>
       </c>
       <c r="G202" t="n">
-        <v>36.36</v>
+        <v>100</v>
       </c>
       <c r="H202" t="n">
         <v>100</v>
@@ -8647,13 +8647,13 @@
       </c>
       <c r="D206" t="inlineStr"/>
       <c r="E206" t="n">
-        <v>65.68000000000001</v>
+        <v>72.5</v>
       </c>
       <c r="F206" t="n">
         <v>0</v>
       </c>
       <c r="G206" t="n">
-        <v>72.73</v>
+        <v>100</v>
       </c>
       <c r="H206" t="n">
         <v>100</v>
@@ -8687,13 +8687,13 @@
         </is>
       </c>
       <c r="E207" t="n">
-        <v>65.68000000000001</v>
+        <v>72.5</v>
       </c>
       <c r="F207" t="n">
         <v>0</v>
       </c>
       <c r="G207" t="n">
-        <v>72.73</v>
+        <v>100</v>
       </c>
       <c r="H207" t="n">
         <v>100</v>
@@ -8727,13 +8727,13 @@
         </is>
       </c>
       <c r="E208" t="n">
-        <v>75.13</v>
+        <v>81.94</v>
       </c>
       <c r="F208" t="n">
         <v>27.78</v>
       </c>
       <c r="G208" t="n">
-        <v>72.73</v>
+        <v>100</v>
       </c>
       <c r="H208" t="n">
         <v>100</v>
@@ -8767,13 +8767,13 @@
         </is>
       </c>
       <c r="E209" t="n">
-        <v>65.68000000000001</v>
+        <v>72.5</v>
       </c>
       <c r="F209" t="n">
         <v>0</v>
       </c>
       <c r="G209" t="n">
-        <v>72.73</v>
+        <v>100</v>
       </c>
       <c r="H209" t="n">
         <v>100</v>
@@ -8807,13 +8807,13 @@
         </is>
       </c>
       <c r="E210" t="n">
-        <v>62.95</v>
+        <v>67.5</v>
       </c>
       <c r="F210" t="n">
         <v>0</v>
       </c>
       <c r="G210" t="n">
-        <v>81.81999999999999</v>
+        <v>100</v>
       </c>
       <c r="H210" t="n">
         <v>100</v>
@@ -8847,13 +8847,13 @@
         </is>
       </c>
       <c r="E211" t="n">
-        <v>65.68000000000001</v>
+        <v>72.5</v>
       </c>
       <c r="F211" t="n">
         <v>0</v>
       </c>
       <c r="G211" t="n">
-        <v>72.73</v>
+        <v>100</v>
       </c>
       <c r="H211" t="n">
         <v>100</v>
@@ -8887,13 +8887,13 @@
         </is>
       </c>
       <c r="E212" t="n">
-        <v>68.18000000000001</v>
+        <v>75</v>
       </c>
       <c r="F212" t="n">
         <v>0</v>
       </c>
       <c r="G212" t="n">
-        <v>72.73</v>
+        <v>100</v>
       </c>
       <c r="H212" t="n">
         <v>100</v>
@@ -8927,13 +8927,13 @@
         </is>
       </c>
       <c r="E213" t="n">
-        <v>62.95</v>
+        <v>67.5</v>
       </c>
       <c r="F213" t="n">
         <v>0</v>
       </c>
       <c r="G213" t="n">
-        <v>81.81999999999999</v>
+        <v>100</v>
       </c>
       <c r="H213" t="n">
         <v>100</v>
@@ -8967,13 +8967,13 @@
         </is>
       </c>
       <c r="E214" t="n">
-        <v>65.68000000000001</v>
+        <v>72.5</v>
       </c>
       <c r="F214" t="n">
         <v>0</v>
       </c>
       <c r="G214" t="n">
-        <v>72.73</v>
+        <v>100</v>
       </c>
       <c r="H214" t="n">
         <v>100</v>

</xml_diff>